<commit_message>
loop through pages to apply jobs
</commit_message>
<xml_diff>
--- a/applied_jobs.xlsx
+++ b/applied_jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amey\python\naukri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0672BC-20F1-4583-B3E5-B8EC2D64C1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7EF621-15B1-420E-B8E4-3B4DB63F14FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
on apply chatbot answer and apply
</commit_message>
<xml_diff>
--- a/applied_jobs.xlsx
+++ b/applied_jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amey\python\naukri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7EF621-15B1-420E-B8E4-3B4DB63F14FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E9DFB7-07C1-41F3-A8E2-DB0273F09875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>